<commit_message>
Tidied directory to keep only the code used for the paper
</commit_message>
<xml_diff>
--- a/envRS_datadict.xlsx
+++ b/envRS_datadict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eilee\Desktop\PhD\Year 3\envRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AF86CD-1F9B-4BB7-B61F-35B24F64717E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427C1472-B52B-45C5-AABA-95DB325FB17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{37A72D85-F0C6-4E36-B57B-427F300141F0}"/>
+    <workbookView xWindow="11450" yWindow="0" windowWidth="7840" windowHeight="10170" xr2:uid="{37A72D85-F0C6-4E36-B57B-427F300141F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="205">
   <si>
     <t>RISK FACTOR</t>
   </si>
@@ -563,9 +563,6 @@
     <t>p_depression</t>
   </si>
   <si>
-    <t>INCLUDED?</t>
-  </si>
-  <si>
     <t>depRS name (if different)</t>
   </si>
   <si>
@@ -639,6 +636,21 @@
   </si>
   <si>
     <t xml:space="preserve">[parent reported] sex at birth. Intersex individuals unfortunately excluded due to small sample size </t>
+  </si>
+  <si>
+    <t>demographics</t>
+  </si>
+  <si>
+    <t>AT BASELINE?</t>
+  </si>
+  <si>
+    <t>AT Y2?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -751,12 +763,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1095,8 +1107,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1109,6 +1122,7 @@
     <col min="6" max="6" width="70.81640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.54296875" customWidth="1"/>
     <col min="8" max="8" width="12.90625" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1122,7 +1136,7 @@
         <v>22</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>89</v>
@@ -1134,964 +1148,1118 @@
         <v>157</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>175</v>
+        <v>201</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" t="s">
         <v>169</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" t="s">
         <v>161</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="H2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" t="s">
         <v>170</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" t="s">
         <v>161</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="H3" t="s">
+        <v>203</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" t="s">
         <v>171</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
+      <c r="H4" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" t="s">
         <v>143</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" t="s">
         <v>172</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="H5" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" t="s">
         <v>147</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" t="s">
         <v>146</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" t="s">
         <v>173</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
+      <c r="H6" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" t="s">
         <v>154</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" t="s">
         <v>155</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" t="s">
         <v>174</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
+      <c r="H7" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
+      <c r="H8" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" t="s">
         <v>117</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11" t="s">
+      <c r="D9"/>
+      <c r="E9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="H9" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" t="s">
         <v>124</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
+      <c r="H10" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" t="s">
+        <v>176</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" t="s">
         <v>177</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" t="s">
+        <v>180</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-    </row>
-    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="E13" s="11" t="s">
+      <c r="F18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" t="s">
+        <v>181</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" t="s">
+        <v>182</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>183</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>184</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" t="s">
+        <v>185</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" t="s">
+        <v>186</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" t="s">
+        <v>187</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" t="s">
+        <v>138</v>
+      </c>
+      <c r="D36" t="s">
+        <v>188</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-    </row>
-    <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E17" s="11" t="s">
+      <c r="F36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" t="s">
+        <v>189</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38"/>
+      <c r="C38" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="F38" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" t="s">
+        <v>190</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B40" t="s">
+        <v>194</v>
+      </c>
+      <c r="C40" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="10" t="s">
+      <c r="D40" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B41" t="s">
+        <v>193</v>
+      </c>
+      <c r="C41" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-    </row>
-    <row r="22" spans="1:9" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-    </row>
-    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-    </row>
-    <row r="24" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-    </row>
-    <row r="26" spans="1:9" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-    </row>
-    <row r="27" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-    </row>
-    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-    </row>
-    <row r="29" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-    </row>
-    <row r="30" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-    </row>
-    <row r="31" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-    </row>
-    <row r="32" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-    </row>
-    <row r="35" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-    </row>
-    <row r="36" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-    </row>
-    <row r="37" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-    </row>
-    <row r="38" spans="1:9" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-    </row>
-    <row r="39" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F39" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-    </row>
-    <row r="40" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="B40" s="10" t="s">
+      <c r="D41" t="s">
         <v>195</v>
       </c>
-      <c r="C40" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="F40" s="11" t="s">
+      <c r="E41" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-    </row>
-    <row r="41" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="E41" s="11" t="s">
+      <c r="F41" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="G41" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
+      <c r="H41" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="I41" s="12" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="42" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="8"/>
@@ -2145,5 +2313,6 @@
     <sortCondition ref="G1:G54"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added longitudinal EN model.
</commit_message>
<xml_diff>
--- a/envRS_datadict.xlsx
+++ b/envRS_datadict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eilee\Desktop\PhD\Year 3\envRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCE03E4-B55F-4CDD-91C3-3DCF26D85860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BBB3BD-74A5-4B89-9D4E-1F6A988A12C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{37A72D85-F0C6-4E36-B57B-427F300141F0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{37A72D85-F0C6-4E36-B57B-427F300141F0}"/>
   </bookViews>
   <sheets>
     <sheet name="included in envRS" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="320">
   <si>
     <t>RISK FACTOR</t>
   </si>
@@ -208,9 +208,6 @@
     <t>[parent-report] witnessed someone shot or stabbed in the community (related to community safety)</t>
   </si>
   <si>
-    <t>[parent-report] endorsed any of the following: ksads_ptsd_raw_764_p, ksads_ptsd_raw_765_p [threated to kill - surely this should be expanded??]</t>
-  </si>
-  <si>
     <t>[parent-report] endorsed any of the following: ksads_ptsd_raw_761_p, ksads_ptsd_raw_762_p, ksads_ptsd_raw_763_p</t>
   </si>
   <si>
@@ -998,6 +995,9 @@
   </si>
   <si>
     <t>[youth-reported] CRPBI - Acceptance Subscale Mean of Report by Parent Completing Protocol by youth. Validation: Minimum of 4 items answered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[parent-report] endorsed any of the following: ksads_ptsd_raw_764_p, ksads_ptsd_raw_765_p </t>
   </si>
 </sst>
 </file>
@@ -1473,7 +1473,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+      <selection pane="topRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1500,22 +1500,22 @@
         <v>21</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1532,16 +1532,16 @@
         <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1558,16 +1558,16 @@
         <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1584,16 +1584,16 @@
         <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>56</v>
+        <v>319</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1607,7 +1607,7 @@
         <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>23</v>
@@ -1616,13 +1616,13 @@
         <v>55</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1636,7 +1636,7 @@
         <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>23</v>
@@ -1645,13 +1645,13 @@
         <v>54</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J6" s="2"/>
     </row>
@@ -1666,7 +1666,7 @@
         <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>23</v>
@@ -1675,13 +1675,13 @@
         <v>52</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
@@ -1701,124 +1701,124 @@
         <v>53</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="54.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
         <v>71</v>
       </c>
-      <c r="B11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" t="s">
-        <v>72</v>
-      </c>
       <c r="E11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
         <v>84</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>85</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J12" s="2"/>
     </row>
@@ -1827,28 +1827,28 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
         <v>88</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D13" t="s">
-        <v>159</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1856,51 +1856,51 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
         <v>60</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C15" t="s">
+      <c r="F15" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J15" s="2"/>
     </row>
@@ -1909,28 +1909,28 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" t="s">
+        <v>154</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -1944,230 +1944,230 @@
         <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J17"/>
     </row>
     <row r="18" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" t="s">
         <v>120</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C18" t="s">
-        <v>121</v>
-      </c>
-      <c r="D18" t="s">
-        <v>149</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J18"/>
     </row>
     <row r="19" spans="1:10" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B19" t="s">
         <v>315</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>317</v>
+      </c>
+      <c r="D19" t="s">
         <v>316</v>
-      </c>
-      <c r="C19" t="s">
-        <v>318</v>
-      </c>
-      <c r="D19" t="s">
-        <v>317</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" t="s">
         <v>124</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C20" t="s">
-        <v>125</v>
-      </c>
-      <c r="D20" t="s">
-        <v>150</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J20"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" t="s">
         <v>132</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>133</v>
       </c>
-      <c r="C21" t="s">
-        <v>134</v>
-      </c>
       <c r="D21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="G22" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" t="s">
         <v>169</v>
       </c>
-      <c r="B23" t="s">
-        <v>170</v>
-      </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="H23" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J23"/>
     </row>
     <row r="24" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" t="s">
         <v>94</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>95</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>165</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D24" t="s">
-        <v>166</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="G24" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2175,54 +2175,54 @@
         <v>13</v>
       </c>
       <c r="C25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" t="s">
         <v>111</v>
-      </c>
-      <c r="D25" t="s">
-        <v>112</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" t="s">
         <v>107</v>
       </c>
-      <c r="B26" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" t="s">
-        <v>108</v>
-      </c>
       <c r="D26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="2" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
@@ -2230,28 +2230,28 @@
         <v>18</v>
       </c>
       <c r="B27" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27" t="s">
         <v>117</v>
       </c>
-      <c r="C27" t="s">
-        <v>118</v>
-      </c>
       <c r="D27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J27"/>
     </row>
@@ -2266,7 +2266,7 @@
         <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>29</v>
@@ -2275,71 +2275,71 @@
         <v>30</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" t="s">
         <v>114</v>
       </c>
-      <c r="B29" t="s">
-        <v>115</v>
-      </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" t="s">
         <v>128</v>
       </c>
-      <c r="C30" t="s">
-        <v>129</v>
-      </c>
       <c r="D30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2353,7 +2353,7 @@
         <v>46</v>
       </c>
       <c r="D31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>47</v>
@@ -2362,13 +2362,13 @@
         <v>50</v>
       </c>
       <c r="G31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J31" s="7"/>
     </row>
@@ -2383,7 +2383,7 @@
         <v>46</v>
       </c>
       <c r="D32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>47</v>
@@ -2392,13 +2392,13 @@
         <v>51</v>
       </c>
       <c r="G32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I32" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J32" s="9"/>
     </row>
@@ -2413,7 +2413,7 @@
         <v>46</v>
       </c>
       <c r="D33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>47</v>
@@ -2422,13 +2422,13 @@
         <v>50</v>
       </c>
       <c r="G33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2442,22 +2442,22 @@
         <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
@@ -2534,63 +2534,63 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B11" s="17"/>
       <c r="D11" s="1"/>
@@ -2639,23 +2639,23 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -2663,7 +2663,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2701,107 +2701,107 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="H1" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>251</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -2809,42 +2809,42 @@
         <v>10</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>297</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -2852,65 +2852,65 @@
         <v>13</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>295</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -2918,65 +2918,65 @@
         <v>6</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>278</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="E12" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>232</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -2984,91 +2984,91 @@
         <v>5</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>253</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>278</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>264</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3076,65 +3076,65 @@
         <v>4</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>278</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B20" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="F20" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -3142,19 +3142,19 @@
         <v>11</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>260</v>
-      </c>
       <c r="G21" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3162,45 +3162,45 @@
         <v>8</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="G22" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="58" x14ac:dyDescent="0.35">
@@ -3208,92 +3208,92 @@
         <v>12</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>270</v>
-      </c>
       <c r="F24" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="G25" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>213</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B26" s="15" t="s">
-        <v>278</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>276</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -3301,22 +3301,22 @@
         <v>1</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -3324,19 +3324,19 @@
         <v>2</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3344,22 +3344,22 @@
         <v>3</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="F30" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3367,42 +3367,42 @@
         <v>7</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>287</v>
-      </c>
       <c r="G32" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -3410,22 +3410,22 @@
         <v>18</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="G33" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H33" s="1"/>
     </row>
@@ -3434,16 +3434,16 @@
         <v>16</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3451,16 +3451,16 @@
         <v>17</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3468,16 +3468,16 @@
         <v>15</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3485,59 +3485,59 @@
         <v>14</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="G39" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>